<commit_message>
cleaned code, separated functions from executions
</commit_message>
<xml_diff>
--- a/TSP/Solutions/IHC.xlsx
+++ b/TSP/Solutions/IHC.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G201"/>
+  <dimension ref="A1:G301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6870,6 +6870,3206 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>[ 8  7  0 21 15 40  2 13 12 24 33 47  4 28  1 41  9  3 25 34 44 23 31 38
+ 20 46 22 10 11 14 32 19 26 16 42 29  5 36 18 27 35 30 37 43 17  6 45 39]</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>12371</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F202" t="n">
+        <v>100</v>
+      </c>
+      <c r="G202" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>[14 10 39  8  0  7 21 15  2 40 33 13  4 47 28  1 41  3 25 34 44  9 23 31
+ 38 24 12 20 19 29 42 16 18 36  5 26 35 27  6 17 45 30 43 37 22 46 11 32]</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>13026</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F203" t="n">
+        <v>100</v>
+      </c>
+      <c r="G203" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>[28  4 47 24 12 46 13 33 22 40  2 21 15  0  7  8 37 30 43 35 19 42 16 36
+ 18 26 29  5 27  6 17 45 32 10 39 14 11 20 38 31 41 23 34 44  9  3 25  1]</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>13203</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F204" t="n">
+        <v>100</v>
+      </c>
+      <c r="G204" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>[16 18 36 26  5  6 43 30 37  8  7  0 15 21 19 32 11 39 10 22 13 46 12 20
+ 24  1 25  3 34 44  9 23 41 31 38 47  4 28 40 33  2 14 45 35 17 27 29 42]</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>13238</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F205" t="n">
+        <v>100</v>
+      </c>
+      <c r="G205" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>[ 6 17 30 37  7  8 39 43 45 32 14 11  0 21 15 40 33  4 47 38 20 31 23 44
+ 34  3 25 41  9  1 28 24 13  2 10 22 12 46 19 35 29 42 26 18 16 36  5 27]</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>13239</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F206" t="n">
+        <v>100</v>
+      </c>
+      <c r="G206" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>[ 4 41  9  3 25 34 44 23 31 38 13 24 47 20 46 12 22  2 10 19 36  5 18 16
+ 26 42 29 27 17 35  6 43 45 32 11 14  8  0  7 37 30 39 21 15 40 33  1 28]</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>13249</v>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F207" t="n">
+        <v>100</v>
+      </c>
+      <c r="G207" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>[43  8 39  2 40 28 41 47  4  1  3 25 34 44 23  9 38 31 20 24 33 15 21  7
+  0 37 30 45 14 11 19 46 12 13 22 10 32 35 17 36 18 26 16 42 29  5 27  6]</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>13336</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F208" t="n">
+        <v>100</v>
+      </c>
+      <c r="G208" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>[36 18 29 17 43 30 37 32 19 46 11 10 22 13 12 20 24 38 31  9 34 44 23  3
+ 25  1 41 47 28  4 33 40  2 14 39 21 15  0  7  8 45 35 27  6  5 42 16 26]</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>13343</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F209" t="n">
+        <v>100</v>
+      </c>
+      <c r="G209" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>[ 1 25  3  9 34 44 23  4 33 40  2 22 14  8 43 17  6 27 36 18  5 26 16 42
+ 29 35 30 37 39 21 15  0  7 45 32 19 11 10 46 20 24 13 12 31 38 47 28 41]</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>13404</v>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F210" t="n">
+        <v>100</v>
+      </c>
+      <c r="G210" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>[41 34  9 44 23 47 28  4 38 31 20 46 12 10 22 39  0  7  8 37 30 43 17  6
+ 45 32 35 27  5 18 36 26 42 16 29 19 11 14 13 24 33  2 21 15 40  1  3 25]</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>13407</v>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F211" t="n">
+        <v>100</v>
+      </c>
+      <c r="G211" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>[ 1 28 24 22  2 40 33 15 21 10 19 46 39  8  0  7 37 30  6 27 29 36 18 42
+ 16 26  5 35 43 17 45 32 14 11 13 12 20 31 38 23  9 41  4 47 44 34  3 25]</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>13517</v>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F212" t="n">
+        <v>100</v>
+      </c>
+      <c r="G212" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>[24 12 22 10  0  7 15 21  2 39  8 37 30 45 43 27 29  5 36 18 16 26 42 35
+  6 17 19 32 14 11 20 46 31 23  9 44 34  3 25  1 41 38 13 47  4 28 40 33]</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>13530</v>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F213" t="n">
+        <v>100</v>
+      </c>
+      <c r="G213" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>[ 1 40 28  4 33 22 21  2 15 39 14 10 13 24 12 11 32 45  7  0  8 37 30 43
+ 17  6 35 27 36 18 26 42 16 29  5 19 46 20 38 31 23 44 34  3 25  9 41 47]</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>13532</v>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F214" t="n">
+        <v>100</v>
+      </c>
+      <c r="G214" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>[32 17 35 36 26 16 18  5 29 42 27 43  6 37 30 45 14  8  7  0 15 21 39 10
+ 22  2 40 33 28  1 41  9 25  3 34 44 23 31 38 13 47  4 46 20 24 12 11 19]</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>13568</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F215" t="n">
+        <v>100</v>
+      </c>
+      <c r="G215" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>[13 22 11 32  6 17 43 35  5 36 18 27 29 26 16 42 19 46 10 14 39 45 30 37
+  8  7 15  0 21  2 33 40 28  1  3 44 34 25 23  9 41  4 47 24 20 38 31 12]</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>13618</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F216" t="n">
+        <v>100</v>
+      </c>
+      <c r="G216" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>[43 17  6  5 29 26 16 42 18 36 35 27 11 10 46 13 24 20 12 22 33 28  4 47
+ 38 31 23 44 34  9  1  3 25 41 40  2 15 21  0  7  8 39 14 37 30 45 19 32]</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>13640</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F217" t="n">
+        <v>100</v>
+      </c>
+      <c r="G217" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>[12 22 10 11 37 30 43 17  6 27 26 16 42 36 18  5 29 35 32 45  8  0  7 15
+ 40  2 13 28  1 25  3 34 44  9 47  4 41 31 23 38 20 46 19 14 39 21 33 24]</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>13727</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F218" t="n">
+        <v>100</v>
+      </c>
+      <c r="G218" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>[12 38 31 47  4 41 34 44 23  9 25  3 28  1 33 24 13 20 46 19 35  6 27  5
+ 17 29 42 16 26 18 36 32 45 43 30 37  7  0  8 14 11 39 21 15  2 40 22 10]</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>13736</v>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F219" t="n">
+        <v>100</v>
+      </c>
+      <c r="G219" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>[15 21  2 40 33 22 12 20 31 38 41 44  3 25 34 23  9 47  4  1 28 24 13 46
+ 11 10 19 32 45 30 37 43 17 27  6  5 18 36 26 16 42 29 35 39 14  8  7  0]</t>
+        </is>
+      </c>
+      <c r="D220" t="n">
+        <v>13763</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F220" t="n">
+        <v>100</v>
+      </c>
+      <c r="G220" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>[ 6 30 37 43 17 45 14 46 39  0  8  7 15 21  2 33 40 28 41  1  4  9 25  3
+ 34 44 23 31 38 47 24 13 12 22 10 20 11 32 19 42 16  5 18 36 26 29 35 27]</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>13884</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F221" t="n">
+        <v>100</v>
+      </c>
+      <c r="G221" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>[23 24 12 13  2 33 40 21 15  7 39 14 32 42 16 26 18 36  5 27 35 45 11 19
+ 29 17  6 43 30 37  8  0 22 10 46 20 31 47  4 28 38 41  1 25  3 34 44  9]</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>13930</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F222" t="n">
+        <v>100</v>
+      </c>
+      <c r="G222" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>[39  8  7 21  0 15  2 13 24 47 41  9 44 25  3 34  1 28 23 31 38  4 33 40
+ 22 12 10 20 46 19 11 32 45 30 37 43 17  6 27  5 36 18 26 16 42 29 35 14]</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>13956</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F223" t="n">
+        <v>100</v>
+      </c>
+      <c r="G223" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>[ 7 15  2 22 12 13 38 31 23  9 44  3 34 25 41 47  4  1 28 40 21 33 24 20
+ 11 19 46 10 14  8 39 37 30 43 17 35 29 42 26 16 18 36  5 27  6 45 32  0]</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>13967</v>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F224" t="n">
+        <v>100</v>
+      </c>
+      <c r="G224" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>[ 9 41 23 47  4 24 21 15 40  2 39 14  0  8  7 37 17 27  6 29 18 36  5 26
+ 42 16 20 31 38 12 46 19 45 43 30 35 32 11 10 22 13 33 28  1  3 25 34 44]</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>13994</v>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F225" t="n">
+        <v>100</v>
+      </c>
+      <c r="G225" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>[47  4 38 31 23  9 41 25 44 34  3  1 13 33  2 22 24 12 46 20 10 11 19 14
+ 39  7  0  8 37 45 43 17 35 26 42 29 16 18 36  5  6 27 30 32 21 15 40 28]</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>14014</v>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F226" t="n">
+        <v>100</v>
+      </c>
+      <c r="G226" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>[24 12 10 22  2 39 21  0  7 37  8 45 30 27 43 17  6 18 26 16 42 29  5 36
+ 35 11 32 14 19 46 20 31 38 47 41 23  9 25 34 44  3  1  4 33 15 40 28 13]</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>14032</v>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F227" t="n">
+        <v>100</v>
+      </c>
+      <c r="G227" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>[38 31 23 44 25  3 34  9 47  4  1 28 41 24 12 13 33  2 15 40 21 39  8 14
+ 32 11 46 19 27 29 36 16 42 26 18  5 35  6 17 45 43 30 37  7  0 22 10 20]</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>14039</v>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F228" t="n">
+        <v>100</v>
+      </c>
+      <c r="G228" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>[ 9 47 23 31 20 38 13 33 40  2 15 21 10 12 46 19 32 45 17 27 35  6  5 29
+ 26 18 36 16 42 11 14 43 30 37  7  0  8 39 22 24 41  4 28  1 25  3 34 44]</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>14043</v>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F229" t="n">
+        <v>100</v>
+      </c>
+      <c r="G229" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>[ 3 34 44 25 41  9 23 31 38 24 12 46 10 22 39 21 33  4 47 20 13 11 17  6
+ 27 36  5 18 16 26 42 29 35 14 32 19 45 43 30 37  8  7  0 15  2 40 28  1]</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>14046</v>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F230" t="n">
+        <v>100</v>
+      </c>
+      <c r="G230" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>[35 27  6 17 29  5 36 18 26 16 42 20 46 12 22 10 11 14 39 45 30 37  8  7
+  0 15 21  2 13 47  4 24 38 31 23 44 34  3 41 25  9  1 28 33 40 19 32 43]</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>14051</v>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F231" t="n">
+        <v>100</v>
+      </c>
+      <c r="G231" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>[ 9 47  4 24 17 35  6 27  5 36 18 16 26 42 29 43 37 30 32 46 20 19 45 14
+ 39  8  7  0 15 21 40 33  2 13 22 10 11 12 38 31 23 41  1 28 25  3 34 44]</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>14066</v>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F232" t="n">
+        <v>100</v>
+      </c>
+      <c r="G232" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>[40 15 22 39  8  2 14 11 12 46 24 33 28  1  3 25 41  9 34 44 23  4 47 38
+ 31 20 19 32 35 29 18 36 26 42 16  5 27  6 17 43 45 30 37  7  0 21 10 13]</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>14074</v>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F233" t="n">
+        <v>100</v>
+      </c>
+      <c r="G233" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>[18 27 42 35  6 43 30 45 32 14 11 10 12 24 13 22 21 15  2 40 25  3  1 34
+ 44  9 23 41 28 33  4 47 31 38 20 46 19 39  0  7  8 37 17 29  5 36 16 26]</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>14123</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F234" t="n">
+        <v>100</v>
+      </c>
+      <c r="G234" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>[23 31 38 20 46 29  5 36 16 18 26 42 32 45 30 43  6 27 35 17 37  7  8 11
+ 14 39 19 10 22  2  0 21 15 40 33 28  1 41  4 13 12 24 47 44 34 25  3  9]</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>14133</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F235" t="n">
+        <v>100</v>
+      </c>
+      <c r="G235" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>[23 13 22 10 39 14 32 35 19 11 27  5 42 26 36 18 16 29  6 43 17 45 37 30
+  8  7  0 15 21  2 40 33 28  1 41  9 44 34 25  3  4 47 38 24 20 46 12 31]</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>14167</v>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F236" t="n">
+        <v>100</v>
+      </c>
+      <c r="G236" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>[44 34 25  3  9 41 33 10 39 14 45 37 30 43 35 11 46 19 42 16 26 18 36  5
+ 29 27 17  6 32 20 24 13 12 22  2  0  8  7 21 15 40  1 28  4 38 31 47 23]</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>14171</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F237" t="n">
+        <v>100</v>
+      </c>
+      <c r="G237" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>[12 10 11 45  6 17 27 36 18 16 42 26 29 35  5 19 32 43 30  7 37  0  8 39
+ 14 46 20 24 47 41 23 38 31  9 44 34  3 25  1 28  4 40 21 15  2 33 22 13]</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>14191</v>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F238" t="n">
+        <v>100</v>
+      </c>
+      <c r="G238" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>[29 42 26 36 18 16  5 35  6 11 10 39 21 15 40 33 38 31 41 25  3 34 44  9
+ 23 47  4 28  1 24  2 12 46 19 20 13 22 14 32 45 43 30 37  7  0  8 17 27]</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>14191</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F239" t="n">
+        <v>100</v>
+      </c>
+      <c r="G239" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>[16 18 36  5 27 35 14 11 10 12 46 19 20 38 31 23 34 44  9 41 47 28 33  2
+ 15 40  1  3 25  4 13 24 22 39  8 21  0  7 37 17  6 43 30 45 32 42 29 26]</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>14199</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F240" t="n">
+        <v>100</v>
+      </c>
+      <c r="G240" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>[11 10 46 20 19 35 27 29 18 16 42 26 36  5 45 32 14 39  0  8  7 21 22 31
+ 38 41  9 34 23 44  3 25  1 28  4 47 24 12 13 33 40 15  2 37 30  6 43 17]</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>14219</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F241" t="n">
+        <v>100</v>
+      </c>
+      <c r="G241" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>[28  4 23 41 47 24 12 20 46 10 14 11 35  6  5 18 36 16 26 42 29 27 17 43
+ 30 45 19 32  8  0  7 37 39 22 21 15 40  1  3 25 44 34  9 38 31 13  2 33]</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>14258</v>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F242" t="n">
+        <v>100</v>
+      </c>
+      <c r="G242" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>[ 0  7 37 30  6 17 11 39 22 13  2 10 21 15 40 33 24  4 47  1 28 25  3 34
+  9 41 44 23 31 38 12 20 46 19 45 43 29 42 16 26  5 18 36 27 35 32 14  8]</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>14265</v>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F243" t="n">
+        <v>100</v>
+      </c>
+      <c r="G243" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>[ 4 47 24 28  1 41 34  3 25 44  9 23 31 38 20 22 13 12 46 10 11 27 35 29
+ 42 26 18 16 36  5 17 19 32 45 14 30  6 43  8 39 37  7  0 21 15  2 40 33]</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>14272</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F244" t="n">
+        <v>100</v>
+      </c>
+      <c r="G244" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>[18  5 26 16 42 29 17 37  0 21  7  8 19 46 22 20 31 38  4 47 28  1 25 41
+  9  3 44 34 23 24 33  2 15 40 13 12 10 11 14 39 32 45 30 43 35 27  6 36]</t>
+        </is>
+      </c>
+      <c r="D245" t="n">
+        <v>14296</v>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F245" t="n">
+        <v>100</v>
+      </c>
+      <c r="G245" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>[45 29 35 26 16 42 36 18  5 27  6 17 43 30 37  0  8  7 15  2 21 22 38 31
+ 25  3 44 34  9 23 41  1 40 28  4 47 33 13 24 12 46 19 39 20 10 11 14 32]</t>
+        </is>
+      </c>
+      <c r="D246" t="n">
+        <v>14297</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F246" t="n">
+        <v>100</v>
+      </c>
+      <c r="G246" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>[42 16 26  5 36 18  6 17 43 30 37  7  0 15 21 14 10 22  2 39  8 40 28  4
+ 33 47 41  1 25  3  9 34 44 31 23 38 20 13 24 12 46 19 32 11 45 35 27 29]</t>
+        </is>
+      </c>
+      <c r="D247" t="n">
+        <v>14321</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F247" t="n">
+        <v>100</v>
+      </c>
+      <c r="G247" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>[11 46 19 35 43 17 29 36 18  5 26 16 42 27  6 30  8 39 45 32 37  7  0 21
+ 15 33 13 23  9 44 34  3 25 41 47 38 20 31 24  4 28  1 40  2 12 22 10 14]</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>14323</v>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F248" t="n">
+        <v>100</v>
+      </c>
+      <c r="G248" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>[23 44 34  9 25  3  1 41 28  4 47 24 46 27  5 26 16 42 18 36 29 35 32  0
+ 21 15 40 33 13  2 39  8  7 37  6 17 19 45 30 43 11 14 10 22 20 12 38 31]</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>14413</v>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F249" t="n">
+        <v>100</v>
+      </c>
+      <c r="G249" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>[43 45 35  6 27  5 18 16 42 26 36 29 19 32 14  8  7  0 21 15  2 39 11 22
+ 13 12 28  1  3 25 34 44 23  9 41 47 40 33  4 46 20 38 31 24 10 37 30 17]</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>14415</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F250" t="n">
+        <v>100</v>
+      </c>
+      <c r="G250" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>[31 38 23 25  3 34 44  9 41 28  1 40  0 15 21 39  8 37  7 30 43 17  6 27
+ 29 18 16 42 26 36  5 32 19 11 12 13  4 47 24 33  2 22 14 35 45 10 46 20]</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>14432</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F251" t="n">
+        <v>100</v>
+      </c>
+      <c r="G251" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>[31 38 12 20 46  1 40 15 21 39 11 14 10 32 19 27 29 36 18 26 16 42  5 35
+  6 17 43 30 45 37  8  7  0  2 22 24 13 33 28  4 25  3 34  9 44 23 41 47]</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>14435</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F252" t="n">
+        <v>100</v>
+      </c>
+      <c r="G252" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>[22 10 19 45 32 30 43 17  6  5 36 18 27 35 29 42 26 16 20 46 13 47 23 31
+ 38 24 12 11 14 39  0  8 37  7 21 15 40  1 44 34  3 25  9 41  4 28 33  2]</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>14455</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F253" t="n">
+        <v>100</v>
+      </c>
+      <c r="G253" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>[17  6 35 42 16 26 18 27 36  5 29 19 11 14 10  2 22 33 12 24 13 28 41 47
+ 38 46 20 31  4 23  9 44 34 25  3  1 40 15 21  7  0 39  8 30 45 32 37 43]</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>14466</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F254" t="n">
+        <v>100</v>
+      </c>
+      <c r="G254" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>[16 42 29 36 18 27 17 35 32 11 19 10 46 12 20 31 38 24 13 33 28  4 47 23
+ 44 34  3 25 41  1  9 40 22 39  2 15 21  7  0 37 14 45 43 30  8  6  5 26]</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>14513</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F255" t="n">
+        <v>100</v>
+      </c>
+      <c r="G255" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>[33 24 31 38  4 47 23 34 44 25  3  9 41 28  1 40 10 20 12 46 19 32 17  6
+ 35 45 14  8 30 37 43  5 27 26 42 16 18 36 29 11 39  7  0 21 15  2 13 22]</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>14540</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F256" t="n">
+        <v>100</v>
+      </c>
+      <c r="G256" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>[30 17  6 27 35 29 16 42 26 18 36  5 19 43 45 32 14 15 21 33 28 40 41  9
+ 23 44 34  3 25  1  4 38 31 47 13 24 12 10 22 20 46 11 39  2  0  7 37  8]</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>14551</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F257" t="n">
+        <v>100</v>
+      </c>
+      <c r="G257" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>[46 19 32 11 39 22  2 15  0  7  8 37 35 27  5 26 36 18 16 42 29  6 17 43
+ 30 45 14 21 40 28  1  4 12 38 20 31 47  3 25 34 44  9 41 23 24 33 13 10]</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>14559</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F258" t="n">
+        <v>100</v>
+      </c>
+      <c r="G258" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>[ 2 13 24 20 31 38 12 46 11 19 10 22 39 37  7  8 30 17 35  6 36 27 29 42
+ 26 18 16  5 43 45 32 14  0 21 15 40 28  1 25  4 41  3 34 44 23  9 47 33]</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>14582</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F259" t="n">
+        <v>100</v>
+      </c>
+      <c r="G259" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>[32 37 27 17 43 30 29  6  5 36 18 16 26 42 35 45  8  7  0 21 15  2 40 33
+  4 28 41  9  1  3 25 34 44 47 23 31 38 20 11 14 39 10 22 13 12 24 46 19]</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>14587</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F260" t="n">
+        <v>100</v>
+      </c>
+      <c r="G260" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>[39 14 37 30 17  6 42 29 27  5 18 16 26 36 35 45 43 32 46 19 11 10 22 20
+ 24 47 41  4 28 13 12 31 38 23  9 34 44  3 25  1 33  2  0 21 15 40  7  8]</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>14591</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F261" t="n">
+        <v>100</v>
+      </c>
+      <c r="G261" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>[ 7  0 21 15 40 13 22  2 33 12 24 47 23 44 34 25  1  4 28  3  9 41 31 38
+ 20 46 10 11 32 19 42 29 36 18 16 26  5 27 35 43  6 30 37 39 17 45 14  8]</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>14604</v>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F262" t="n">
+        <v>100</v>
+      </c>
+      <c r="G262" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>[ 2 47  4 41 23 44 34  3  9 28  1 25 31 38 22 10 39 14 19 32 11 45 37  7
+  0  8 30 43  6 27 35  5 36 42 16 26 18 29 17 46 20 24 13 12 33 40 15 21]</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>14607</v>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F263" t="n">
+        <v>100</v>
+      </c>
+      <c r="G263" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>[22 13  2 21  7  8  0 39 14 32 19 29 42 26 16 18 36 27  6 43 30 45 37 17
+  5 35 11 10 46 20 47 31 38 12 24  4 41 25  3 23 44 34  9  1 28 33 15 40]</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>14614</v>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F264" t="n">
+        <v>100</v>
+      </c>
+      <c r="G264" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>[16 18 36 17 30 37  8  7 21 15 40 13 33  4 47 28  1 23 41  9 34 44  3 25
+ 31 38 12 46 19 11 32 27  5 29  6 35 43 45 14 39  0  2 10 22 24 20 42 26]</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>14671</v>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F265" t="n">
+        <v>100</v>
+      </c>
+      <c r="G265" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>[45 37  0 15 21 40 33  1 25  3 34 44  9 23 38  4 41 31 47 28 24 12 46 10
+ 22 20 13  2 11 32 14 39  7  8 30  6 17 43 35 27 29 36  5 18 26 16 42 19]</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>14678</v>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F266" t="n">
+        <v>100</v>
+      </c>
+      <c r="G266" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>[28  1 41 25  3  9 47 33  4 40  2 21 15 11 32 39  8  0  7 37 17 43 27  6
+ 36 26 42 16 18  5 29 35 30 45 14 19 46 10 22 13 12 20 24 38 31 23 34 44]</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>14680</v>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F267" t="n">
+        <v>100</v>
+      </c>
+      <c r="G267" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>[18  5 36 35 45 43 17  6 27 37 30  8  7  0 39 14 11 46 12 10 22  2 21 15
+ 40 33 28  1  4 31  9 23 34  3 44 25 41 47 38 13 24 20 32 19 29 16 42 26]</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>14697</v>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F268" t="n">
+        <v>100</v>
+      </c>
+      <c r="G268" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>[44  3 28  1 33 40 21  2 22 10 19 46 45 43 17 35 42 16 18 26 29  5 27 36
+  6 30 37  7  0 15 39  8 14 11 32 20 12 13 24 47  4 41 23 31 38  9 25 34]</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>14717</v>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F269" t="n">
+        <v>100</v>
+      </c>
+      <c r="G269" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>[21 15  7  0  8  2 33 13 22 12 24 20 31 44 34  3 25  9 41 23  4 40  1 28
+ 47 38 10 46 19 32 35 29 26 36 18 16 42  5 27  6 30 43 45 14 11 17 37 39]</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>14744</v>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F270" t="n">
+        <v>100</v>
+      </c>
+      <c r="G270" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>[22 10 11 19 29 26 42 16 18 36 27 35  5  6 17 43 32 30 45 37  7  8  0 21
+ 15 40  2 46 20 12 24 31 41  1 25 34  3 44  9 23 47 38  4 28 33 13 14 39]</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>14752</v>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F271" t="n">
+        <v>100</v>
+      </c>
+      <c r="G271" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>[26 18 27  5 42 19 46 20 31 38 13  2 33 28 47  4 25  3  1 41 23 44 34  9
+ 24 12 40 21 15  7  0  8 14 39 10 22 11 32 45 37 30 43 35 36 17  6 29 16]</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>14774</v>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F272" t="n">
+        <v>100</v>
+      </c>
+      <c r="G272" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>[24 13 33 20 38 31 41 23 47  4  9 44 34 25  3  1 28 40 15  0  7 37  8 30
+ 43 17 29  6 27 36 18  5 35 45 14 21 39  2 22 10 32 11 42 16 26 19 46 12]</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>14783</v>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F273" t="n">
+        <v>100</v>
+      </c>
+      <c r="G273" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>[34 44  9 23  4 28 24 13 10 14 32 17 29 35 27 26 19 42 16 18 36  5  6 43
+ 37 30 45 11 22 12 20 46 31 38 47 40 15 21  0  7  8 39  2 33  1 41 25  3]</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>14818</v>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F274" t="n">
+        <v>100</v>
+      </c>
+      <c r="G274" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>[10 32 19 46 31 38 24 22 11 21 15  7  0  8 37 42 29 26 36 18 16  5 35 17
+ 27  6 43 30 45 14 39 40  2 33 28 41 25  3 34 23 44  9  1  4 47 13 12 20]</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>14819</v>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F275" t="n">
+        <v>100</v>
+      </c>
+      <c r="G275" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>[22 10  2 40 33 24 47  9  1  3 34 44 25 23  4 28 41 31 38 20 46 19 42 16
+ 18 26 36  5 17 30 37  7 21 15  0  8 39 14 45 43  6 27 29 35 32 11 12 13]</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>14828</v>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F276" t="n">
+        <v>100</v>
+      </c>
+      <c r="G276" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>[15  2 33 28  1  3 34  9 23 44 25 47 38 31  4 41 24 46 19 14 39 10 11 32
+ 17 35 27 29 42 16 26 18 36  5  6 43 30 45  8 37  7  0 21 20 12 22 13 40]</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>14885</v>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F277" t="n">
+        <v>100</v>
+      </c>
+      <c r="G277" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>[27  6 35  5 18 26 16 42 37  8 14 39  0  7 15 21  2 22 10 12 13 40 33 28
+  3 25 44 34  9 41  1  4 47 23 31 24 38 20 46 32 45 19 11 29 30 43 17 36]</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>14893</v>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F278" t="n">
+        <v>100</v>
+      </c>
+      <c r="G278" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>[16 29 35 45 30  7  0 39 14 10 46 19 11 12 20 31 41  1 28 33  4 47 23  9
+ 34 44 25  3 38 24 13 22 21 15 40  2  8 37 43 17 32 42 18 36  6 27  5 26]</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>14938</v>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F279" t="n">
+        <v>100</v>
+      </c>
+      <c r="G279" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>[18 16 42  5 27 19 11 46 20 12 10 39  0 21 33  4 47 41 25 28  1  3  9 34
+ 44 23 38 31 24 13 22  2 40 15  7 37 32 14 45 17 43 30  8 29 35  6 26 36]</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>14951</v>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F280" t="n">
+        <v>100</v>
+      </c>
+      <c r="G280" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>[13 38 40  1 41  9 44 34  3 25 28  4 47 23 46 19 43 17  6 35 29 42 26 36
+ 18 16  5 27 45 32 30 37  7  0 21 15 39  8 14 11 10 22  2 33 12 31 20 24]</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>14969</v>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F281" t="n">
+        <v>100</v>
+      </c>
+      <c r="G281" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>[19 39 14 45 35  5 30 37  7  8  0 15 40 33 21  2 22 10 46 12 24 13 47 38
+ 28  3 25  9 44 34 23 41  1  4 31 20 11  6 27 16 18 36 26 42 29 17 43 32]</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F282" t="n">
+        <v>100</v>
+      </c>
+      <c r="G282" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>[42 29 19 11 10 22 46 12 20 31 23 41 25 44 34 28 40  1  3  9  4 47 38 13
+ 24 33  2 15 21 14 45 32 35 17 43 37  7  0 39  8 30  6 27  5 18 26 36 16]</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>15006</v>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F283" t="n">
+        <v>100</v>
+      </c>
+      <c r="G283" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>[33 21 39 30 43 17  6 27  5 45 14 32 46 11 20 31 41 25  1  3 34 44  9 23
+ 28  4 47 38 24  2 22 13 12 10 19 29 42 16 36 18 26 35 37  8  0  7 15 40]</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>15021</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F284" t="n">
+        <v>100</v>
+      </c>
+      <c r="G284" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>[ 8 37  6 36 18 26 42 16 29 35  5 27 17 45 11 21 15  2  0  7 30 43 14 32
+ 19 46 20 12 24  4 33 40  1 28  3 25 41 47 44 34  9 23 31 38 22 13 10 39]</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>15063</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F285" t="n">
+        <v>100</v>
+      </c>
+      <c r="G285" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>[ 9  3  1 25 47 33 13 22 11 45 39  8  7  0 15 21  2 40 10 14 32 17 30 37
+ 43  6 35 27 29 18  5 36 16 26 42 19 46 12 24 20 38 31 23 41  4 28 44 34]</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>15086</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F286" t="n">
+        <v>100</v>
+      </c>
+      <c r="G286" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>[26  5 36 18 35 30 45 14 39  0  7 37  8 21 15  2 22 11 10 19 12 24 47 23
+ 38 13 33 40 28  4  9 44  3 25 34  1 41 31 20 46 32 43 17 27  6 29 42 16]</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>15117</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F287" t="n">
+        <v>100</v>
+      </c>
+      <c r="G287" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>[29 27  6 35 19 46 10  2 40 28  3 25 44  9 34 23 41 31 38  4 47  1 33 15
+ 21  8 37 45 30 17 43  7  0 39 14 11 12 20 24 13 22 32 42 16 26 18 36  5]</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>15182</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F288" t="n">
+        <v>100</v>
+      </c>
+      <c r="G288" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>[28 25  3 34  9 31 38 22 10 46 20 19 27 29 42 26 36 18 16  5 35 30  6 17
+ 45 43 37  8 32 11 14 39 21  7  0 15  2 13 24 12 33 40  4 47 41 23 44  1]</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>15194</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F289" t="n">
+        <v>100</v>
+      </c>
+      <c r="G289" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>[37 30 43 45 14 11 19 29  5 42 16 26 18 36  6 27 17 35 10 22 24 12 13 33
+ 38 46 20 31 44  4 47 23 41  9 34  3 25  1 28 40 15  8 39 32  2 21  0  7]</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>15199</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F290" t="n">
+        <v>100</v>
+      </c>
+      <c r="G290" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>[ 3 25  9 23 41  4 38 47 24 13 12 22 33 28 40 15  0  8  7 21  2 11 10 14
+ 32 16 18 36 35  5 29 42 26 27 45 43  6 17 30 37 39 19 46 20 31  1 44 34]</t>
+        </is>
+      </c>
+      <c r="D291" t="n">
+        <v>15220</v>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F291" t="n">
+        <v>100</v>
+      </c>
+      <c r="G291" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>[30 45 39 11 20 24 13 22 46 10 12 38 31 23  4 25  3 34  9 44 47  1 41 28
+ 40 33 15 21  2  0  8  7 37 14 32 19 26 42 16 18 36 29 17  5 27  6 35 43]</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>15235</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F292" t="n">
+        <v>100</v>
+      </c>
+      <c r="G292" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>[13 12 39 14 10 22 46 19 32 11 35 17  5 27 29 26 18 16 42 36  6 43 37 30
+ 45 15  7  8 21  0  2 33 20 38 31 23 47  9 34 44  3 25  1 41  4 28 40 24]</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>15270</v>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F293" t="n">
+        <v>100</v>
+      </c>
+      <c r="G293" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>[21  8  0  7 14 39 37 30 43  6 35 29 27 17 45 32 11 22 33 28 40  1 25  9
+ 23  4 47  3 34 44 41 38 31 20 42 26 16 18 36  5 19 46 12 24 13 10  2 15]</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>15419</v>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F294" t="n">
+        <v>100</v>
+      </c>
+      <c r="G294" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>[ 6 30 35 36 29 26 42 16 18  5 32 21 15 40  1 28 47  4 41 25  3 34 38 31
+ 23 44  9 20 46 12 24 13 33  2  0  7  8 37 43 17 45 11 10 22 39 14 19 27]</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>15428</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F295" t="n">
+        <v>100</v>
+      </c>
+      <c r="G295" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>[10 22 12 13  2 33 28 41  1  9 25  3 23 44 34 31  4 47 38 20 24 46 40 15
+ 21  0 37 45 32 14 11 19 35 36 29 42 16 26 18  5 27 43 17  6  8  7 30 39]</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>15470</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F296" t="n">
+        <v>100</v>
+      </c>
+      <c r="G296" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>[19  6 43 30 37  7 45 32 11 46 13 24 10 22 28  1 41  3 34 44 23 31 38 20
+ 12  4  9 25 47 33  2 40 15 21  0 14 39  8 17 35 27  5 26 36 18 16 42 29]</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>15575</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F297" t="n">
+        <v>100</v>
+      </c>
+      <c r="G297" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>[47 31 23  1 41  9 34 25 44  3  4 28 33 22 12 13 24 10 20 46 35 29  5 27
+ 43 17  6 18 36 26 16 42 19 11 37 30 45 14 32 39  8  7  0 21  2 15 40 38]</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>15894</v>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F298" t="n">
+        <v>100</v>
+      </c>
+      <c r="G298" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>[16 26 18 29 43 37 30  0  2 21 15  1 28 40 33  4 22 12 46 45 32 14 20 38
+ 31 23 41 25  3  9 44 34 47 24 13 10 39  8  7 11 19 35 17  6 36  5 27 42]</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>16083</v>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F299" t="n">
+        <v>100</v>
+      </c>
+      <c r="G299" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>[22 13  2  0  7 15 40 33 28  1 44 34  3  9 38 24 47  4 25 23 41 31 20 19
+ 14 39 21  8 37 30 45 35 18 16 26 42 27 36  5  6 29 17 43 32 46 12 11 10]</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>16223</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F300" t="n">
+        <v>100</v>
+      </c>
+      <c r="G300" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>IHC</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>48 miast</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>[36 17 37 45  6 43 35 30 39 21  0  7  8 15  2  1 40 28 31 20 10 11 19 12
+ 24 13  4 47 41 25  3 34 44  9 23 38 33 22 46 14 32 29  5 27 42 16 26 18]</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>16313</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>Zamiana</t>
+        </is>
+      </c>
+      <c r="F301" t="n">
+        <v>100</v>
+      </c>
+      <c r="G301" t="n">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>